<commit_message>
telegram bot final implementation
</commit_message>
<xml_diff>
--- a/bridge/database/export/acquisizioni.xlsx
+++ b/bridge/database/export/acquisizioni.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="535">
   <si>
     <t>id</t>
   </si>
@@ -1259,6 +1259,366 @@
   </si>
   <si>
     <t>2021-02-13 14:53:28.627932</t>
+  </si>
+  <si>
+    <t>10782</t>
+  </si>
+  <si>
+    <t>2021-02-13 14:53:30.630706</t>
+  </si>
+  <si>
+    <t>10783</t>
+  </si>
+  <si>
+    <t>2021-02-13 14:53:32.63344</t>
+  </si>
+  <si>
+    <t>10784</t>
+  </si>
+  <si>
+    <t>2021-02-13 14:53:34.636232</t>
+  </si>
+  <si>
+    <t>10785</t>
+  </si>
+  <si>
+    <t>2021-02-13 14:53:36.634907</t>
+  </si>
+  <si>
+    <t>10786</t>
+  </si>
+  <si>
+    <t>2021-02-13 14:53:38.637798</t>
+  </si>
+  <si>
+    <t>10787</t>
+  </si>
+  <si>
+    <t>2021-02-13 14:53:40.641136</t>
+  </si>
+  <si>
+    <t>10788</t>
+  </si>
+  <si>
+    <t>2021-02-13 14:53:42.643921</t>
+  </si>
+  <si>
+    <t>10789</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:09.549343</t>
+  </si>
+  <si>
+    <t>10790</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:11.551304</t>
+  </si>
+  <si>
+    <t>10791</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:13.555027</t>
+  </si>
+  <si>
+    <t>10792</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:15.557398</t>
+  </si>
+  <si>
+    <t>10793</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:17.560862</t>
+  </si>
+  <si>
+    <t>10794</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:19.559298</t>
+  </si>
+  <si>
+    <t>10795</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:21.562332</t>
+  </si>
+  <si>
+    <t>10796</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:23.56549</t>
+  </si>
+  <si>
+    <t>10797</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:25.567477</t>
+  </si>
+  <si>
+    <t>10798</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:27.570353</t>
+  </si>
+  <si>
+    <t>10799</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:29.573708</t>
+  </si>
+  <si>
+    <t>10800</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:31.572479</t>
+  </si>
+  <si>
+    <t>10801</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:33.575704</t>
+  </si>
+  <si>
+    <t>10802</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:35.578111</t>
+  </si>
+  <si>
+    <t>10803</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:37.580645</t>
+  </si>
+  <si>
+    <t>10804</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:39.584043</t>
+  </si>
+  <si>
+    <t>10805</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:41.582092</t>
+  </si>
+  <si>
+    <t>10806</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:43.58515</t>
+  </si>
+  <si>
+    <t>10807</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:45.588249</t>
+  </si>
+  <si>
+    <t>10808</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:47.590577</t>
+  </si>
+  <si>
+    <t>10809</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:49.59432</t>
+  </si>
+  <si>
+    <t>10810</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:51.597036</t>
+  </si>
+  <si>
+    <t>10811</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:53.599159</t>
+  </si>
+  <si>
+    <t>10812</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:55.598153</t>
+  </si>
+  <si>
+    <t>10813</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:57.601133</t>
+  </si>
+  <si>
+    <t>10814</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:00:59.604216</t>
+  </si>
+  <si>
+    <t>10815</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:01.606426</t>
+  </si>
+  <si>
+    <t>10816</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:03.606045</t>
+  </si>
+  <si>
+    <t>10817</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:10.125761</t>
+  </si>
+  <si>
+    <t>10818</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:12.124981</t>
+  </si>
+  <si>
+    <t>10819</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:14.12784</t>
+  </si>
+  <si>
+    <t>10820</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:16.130876</t>
+  </si>
+  <si>
+    <t>10821</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:18.132866</t>
+  </si>
+  <si>
+    <t>10822</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:20.131884</t>
+  </si>
+  <si>
+    <t>10823</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:22.135241</t>
+  </si>
+  <si>
+    <t>10824</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:24.138152</t>
+  </si>
+  <si>
+    <t>10825</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:26.140949</t>
+  </si>
+  <si>
+    <t>10826</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:28.142976</t>
+  </si>
+  <si>
+    <t>10827</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:30.145993</t>
+  </si>
+  <si>
+    <t>10828</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:32.149358</t>
+  </si>
+  <si>
+    <t>10829</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:34.148294</t>
+  </si>
+  <si>
+    <t>10830</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:36.151033</t>
+  </si>
+  <si>
+    <t>10831</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:38.153949</t>
+  </si>
+  <si>
+    <t>10832</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:40.156507</t>
+  </si>
+  <si>
+    <t>10833</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:42.155567</t>
+  </si>
+  <si>
+    <t>10834</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:44.157485</t>
+  </si>
+  <si>
+    <t>10835</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:46.160577</t>
+  </si>
+  <si>
+    <t>10836</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:48.163919</t>
+  </si>
+  <si>
+    <t>10837</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:50.166747</t>
+  </si>
+  <si>
+    <t>10838</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:52.16888</t>
+  </si>
+  <si>
+    <t>10839</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:54.172467</t>
+  </si>
+  <si>
+    <t>10840</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:56.170913</t>
+  </si>
+  <si>
+    <t>10841</t>
+  </si>
+  <si>
+    <t>2021-02-13 15:01:58.174102</t>
   </si>
 </sst>
 </file>
@@ -1590,7 +1950,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:I220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6236,6 +6596,1746 @@
         <v>16</v>
       </c>
     </row>
+    <row r="161" spans="1:9">
+      <c r="A161" t="s">
+        <v>415</v>
+      </c>
+      <c r="B161" t="s">
+        <v>416</v>
+      </c>
+      <c r="C161" t="s">
+        <v>209</v>
+      </c>
+      <c r="D161" t="s">
+        <v>210</v>
+      </c>
+      <c r="E161" t="s">
+        <v>211</v>
+      </c>
+      <c r="F161" t="s">
+        <v>223</v>
+      </c>
+      <c r="G161" t="s">
+        <v>218</v>
+      </c>
+      <c r="H161" t="s">
+        <v>223</v>
+      </c>
+      <c r="I161" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9">
+      <c r="A162" t="s">
+        <v>417</v>
+      </c>
+      <c r="B162" t="s">
+        <v>418</v>
+      </c>
+      <c r="C162" t="s">
+        <v>209</v>
+      </c>
+      <c r="D162" t="s">
+        <v>217</v>
+      </c>
+      <c r="E162" t="s">
+        <v>211</v>
+      </c>
+      <c r="F162" t="s">
+        <v>223</v>
+      </c>
+      <c r="G162" t="s">
+        <v>218</v>
+      </c>
+      <c r="H162" t="s">
+        <v>223</v>
+      </c>
+      <c r="I162" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9">
+      <c r="A163" t="s">
+        <v>419</v>
+      </c>
+      <c r="B163" t="s">
+        <v>420</v>
+      </c>
+      <c r="C163" t="s">
+        <v>209</v>
+      </c>
+      <c r="D163" t="s">
+        <v>217</v>
+      </c>
+      <c r="E163" t="s">
+        <v>272</v>
+      </c>
+      <c r="F163" t="s">
+        <v>223</v>
+      </c>
+      <c r="G163" t="s">
+        <v>218</v>
+      </c>
+      <c r="H163" t="s">
+        <v>223</v>
+      </c>
+      <c r="I163" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9">
+      <c r="A164" t="s">
+        <v>421</v>
+      </c>
+      <c r="B164" t="s">
+        <v>422</v>
+      </c>
+      <c r="C164" t="s">
+        <v>209</v>
+      </c>
+      <c r="D164" t="s">
+        <v>217</v>
+      </c>
+      <c r="E164" t="s">
+        <v>211</v>
+      </c>
+      <c r="F164" t="s">
+        <v>258</v>
+      </c>
+      <c r="G164" t="s">
+        <v>218</v>
+      </c>
+      <c r="H164" t="s">
+        <v>223</v>
+      </c>
+      <c r="I164" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
+      <c r="A165" t="s">
+        <v>423</v>
+      </c>
+      <c r="B165" t="s">
+        <v>424</v>
+      </c>
+      <c r="C165" t="s">
+        <v>209</v>
+      </c>
+      <c r="D165" t="s">
+        <v>217</v>
+      </c>
+      <c r="E165" t="s">
+        <v>211</v>
+      </c>
+      <c r="F165" t="s">
+        <v>223</v>
+      </c>
+      <c r="G165" t="s">
+        <v>218</v>
+      </c>
+      <c r="H165" t="s">
+        <v>223</v>
+      </c>
+      <c r="I165" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9">
+      <c r="A166" t="s">
+        <v>425</v>
+      </c>
+      <c r="B166" t="s">
+        <v>426</v>
+      </c>
+      <c r="C166" t="s">
+        <v>209</v>
+      </c>
+      <c r="D166" t="s">
+        <v>217</v>
+      </c>
+      <c r="E166" t="s">
+        <v>211</v>
+      </c>
+      <c r="F166" t="s">
+        <v>223</v>
+      </c>
+      <c r="G166" t="s">
+        <v>218</v>
+      </c>
+      <c r="H166" t="s">
+        <v>223</v>
+      </c>
+      <c r="I166" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9">
+      <c r="A167" t="s">
+        <v>427</v>
+      </c>
+      <c r="B167" t="s">
+        <v>428</v>
+      </c>
+      <c r="C167" t="s">
+        <v>216</v>
+      </c>
+      <c r="D167" t="s">
+        <v>217</v>
+      </c>
+      <c r="E167" t="s">
+        <v>211</v>
+      </c>
+      <c r="F167" t="s">
+        <v>212</v>
+      </c>
+      <c r="G167" t="s">
+        <v>218</v>
+      </c>
+      <c r="H167" t="s">
+        <v>223</v>
+      </c>
+      <c r="I167" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9">
+      <c r="A168" t="s">
+        <v>429</v>
+      </c>
+      <c r="B168" t="s">
+        <v>430</v>
+      </c>
+      <c r="C168" t="s">
+        <v>209</v>
+      </c>
+      <c r="D168" t="s">
+        <v>217</v>
+      </c>
+      <c r="E168" t="s">
+        <v>211</v>
+      </c>
+      <c r="F168" t="s">
+        <v>223</v>
+      </c>
+      <c r="G168" t="s">
+        <v>218</v>
+      </c>
+      <c r="H168" t="s">
+        <v>223</v>
+      </c>
+      <c r="I168" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9">
+      <c r="A169" t="s">
+        <v>431</v>
+      </c>
+      <c r="B169" t="s">
+        <v>432</v>
+      </c>
+      <c r="C169" t="s">
+        <v>209</v>
+      </c>
+      <c r="D169" t="s">
+        <v>210</v>
+      </c>
+      <c r="E169" t="s">
+        <v>211</v>
+      </c>
+      <c r="F169" t="s">
+        <v>223</v>
+      </c>
+      <c r="G169" t="s">
+        <v>218</v>
+      </c>
+      <c r="H169" t="s">
+        <v>223</v>
+      </c>
+      <c r="I169" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9">
+      <c r="A170" t="s">
+        <v>433</v>
+      </c>
+      <c r="B170" t="s">
+        <v>434</v>
+      </c>
+      <c r="C170" t="s">
+        <v>209</v>
+      </c>
+      <c r="D170" t="s">
+        <v>217</v>
+      </c>
+      <c r="E170" t="s">
+        <v>272</v>
+      </c>
+      <c r="F170" t="s">
+        <v>223</v>
+      </c>
+      <c r="G170" t="s">
+        <v>213</v>
+      </c>
+      <c r="H170" t="s">
+        <v>223</v>
+      </c>
+      <c r="I170" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
+      <c r="A171" t="s">
+        <v>435</v>
+      </c>
+      <c r="B171" t="s">
+        <v>436</v>
+      </c>
+      <c r="C171" t="s">
+        <v>209</v>
+      </c>
+      <c r="D171" t="s">
+        <v>217</v>
+      </c>
+      <c r="E171" t="s">
+        <v>211</v>
+      </c>
+      <c r="F171" t="s">
+        <v>223</v>
+      </c>
+      <c r="G171" t="s">
+        <v>218</v>
+      </c>
+      <c r="H171" t="s">
+        <v>223</v>
+      </c>
+      <c r="I171" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="A172" t="s">
+        <v>437</v>
+      </c>
+      <c r="B172" t="s">
+        <v>438</v>
+      </c>
+      <c r="C172" t="s">
+        <v>209</v>
+      </c>
+      <c r="D172" t="s">
+        <v>257</v>
+      </c>
+      <c r="E172" t="s">
+        <v>211</v>
+      </c>
+      <c r="F172" t="s">
+        <v>223</v>
+      </c>
+      <c r="G172" t="s">
+        <v>213</v>
+      </c>
+      <c r="H172" t="s">
+        <v>223</v>
+      </c>
+      <c r="I172" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
+      <c r="A173" t="s">
+        <v>439</v>
+      </c>
+      <c r="B173" t="s">
+        <v>440</v>
+      </c>
+      <c r="C173" t="s">
+        <v>209</v>
+      </c>
+      <c r="D173" t="s">
+        <v>217</v>
+      </c>
+      <c r="E173" t="s">
+        <v>211</v>
+      </c>
+      <c r="F173" t="s">
+        <v>212</v>
+      </c>
+      <c r="G173" t="s">
+        <v>218</v>
+      </c>
+      <c r="H173" t="s">
+        <v>223</v>
+      </c>
+      <c r="I173" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9">
+      <c r="A174" t="s">
+        <v>441</v>
+      </c>
+      <c r="B174" t="s">
+        <v>442</v>
+      </c>
+      <c r="C174" t="s">
+        <v>209</v>
+      </c>
+      <c r="D174" t="s">
+        <v>217</v>
+      </c>
+      <c r="E174" t="s">
+        <v>211</v>
+      </c>
+      <c r="F174" t="s">
+        <v>223</v>
+      </c>
+      <c r="G174" t="s">
+        <v>218</v>
+      </c>
+      <c r="H174" t="s">
+        <v>223</v>
+      </c>
+      <c r="I174" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9">
+      <c r="A175" t="s">
+        <v>443</v>
+      </c>
+      <c r="B175" t="s">
+        <v>444</v>
+      </c>
+      <c r="C175" t="s">
+        <v>209</v>
+      </c>
+      <c r="D175" t="s">
+        <v>217</v>
+      </c>
+      <c r="E175" t="s">
+        <v>211</v>
+      </c>
+      <c r="F175" t="s">
+        <v>223</v>
+      </c>
+      <c r="G175" t="s">
+        <v>218</v>
+      </c>
+      <c r="H175" t="s">
+        <v>212</v>
+      </c>
+      <c r="I175" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9">
+      <c r="A176" t="s">
+        <v>445</v>
+      </c>
+      <c r="B176" t="s">
+        <v>446</v>
+      </c>
+      <c r="C176" t="s">
+        <v>209</v>
+      </c>
+      <c r="D176" t="s">
+        <v>257</v>
+      </c>
+      <c r="E176" t="s">
+        <v>211</v>
+      </c>
+      <c r="F176" t="s">
+        <v>223</v>
+      </c>
+      <c r="G176" t="s">
+        <v>218</v>
+      </c>
+      <c r="H176" t="s">
+        <v>223</v>
+      </c>
+      <c r="I176" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9">
+      <c r="A177" t="s">
+        <v>447</v>
+      </c>
+      <c r="B177" t="s">
+        <v>448</v>
+      </c>
+      <c r="C177" t="s">
+        <v>209</v>
+      </c>
+      <c r="D177" t="s">
+        <v>217</v>
+      </c>
+      <c r="E177" t="s">
+        <v>211</v>
+      </c>
+      <c r="F177" t="s">
+        <v>223</v>
+      </c>
+      <c r="G177" t="s">
+        <v>218</v>
+      </c>
+      <c r="H177" t="s">
+        <v>223</v>
+      </c>
+      <c r="I177" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9">
+      <c r="A178" t="s">
+        <v>449</v>
+      </c>
+      <c r="B178" t="s">
+        <v>450</v>
+      </c>
+      <c r="C178" t="s">
+        <v>209</v>
+      </c>
+      <c r="D178" t="s">
+        <v>217</v>
+      </c>
+      <c r="E178" t="s">
+        <v>211</v>
+      </c>
+      <c r="F178" t="s">
+        <v>212</v>
+      </c>
+      <c r="G178" t="s">
+        <v>218</v>
+      </c>
+      <c r="H178" t="s">
+        <v>212</v>
+      </c>
+      <c r="I178" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9">
+      <c r="A179" t="s">
+        <v>451</v>
+      </c>
+      <c r="B179" t="s">
+        <v>452</v>
+      </c>
+      <c r="C179" t="s">
+        <v>209</v>
+      </c>
+      <c r="D179" t="s">
+        <v>217</v>
+      </c>
+      <c r="E179" t="s">
+        <v>211</v>
+      </c>
+      <c r="F179" t="s">
+        <v>212</v>
+      </c>
+      <c r="G179" t="s">
+        <v>218</v>
+      </c>
+      <c r="H179" t="s">
+        <v>223</v>
+      </c>
+      <c r="I179" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9">
+      <c r="A180" t="s">
+        <v>453</v>
+      </c>
+      <c r="B180" t="s">
+        <v>454</v>
+      </c>
+      <c r="C180" t="s">
+        <v>265</v>
+      </c>
+      <c r="D180" t="s">
+        <v>217</v>
+      </c>
+      <c r="E180" t="s">
+        <v>211</v>
+      </c>
+      <c r="F180" t="s">
+        <v>223</v>
+      </c>
+      <c r="G180" t="s">
+        <v>218</v>
+      </c>
+      <c r="H180" t="s">
+        <v>223</v>
+      </c>
+      <c r="I180" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9">
+      <c r="A181" t="s">
+        <v>455</v>
+      </c>
+      <c r="B181" t="s">
+        <v>456</v>
+      </c>
+      <c r="C181" t="s">
+        <v>209</v>
+      </c>
+      <c r="D181" t="s">
+        <v>217</v>
+      </c>
+      <c r="E181" t="s">
+        <v>211</v>
+      </c>
+      <c r="F181" t="s">
+        <v>223</v>
+      </c>
+      <c r="G181" t="s">
+        <v>213</v>
+      </c>
+      <c r="H181" t="s">
+        <v>223</v>
+      </c>
+      <c r="I181" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9">
+      <c r="A182" t="s">
+        <v>457</v>
+      </c>
+      <c r="B182" t="s">
+        <v>458</v>
+      </c>
+      <c r="C182" t="s">
+        <v>209</v>
+      </c>
+      <c r="D182" t="s">
+        <v>217</v>
+      </c>
+      <c r="E182" t="s">
+        <v>211</v>
+      </c>
+      <c r="F182" t="s">
+        <v>212</v>
+      </c>
+      <c r="G182" t="s">
+        <v>218</v>
+      </c>
+      <c r="H182" t="s">
+        <v>223</v>
+      </c>
+      <c r="I182" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9">
+      <c r="A183" t="s">
+        <v>459</v>
+      </c>
+      <c r="B183" t="s">
+        <v>460</v>
+      </c>
+      <c r="C183" t="s">
+        <v>209</v>
+      </c>
+      <c r="D183" t="s">
+        <v>217</v>
+      </c>
+      <c r="E183" t="s">
+        <v>211</v>
+      </c>
+      <c r="F183" t="s">
+        <v>223</v>
+      </c>
+      <c r="G183" t="s">
+        <v>218</v>
+      </c>
+      <c r="H183" t="s">
+        <v>223</v>
+      </c>
+      <c r="I183" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9">
+      <c r="A184" t="s">
+        <v>461</v>
+      </c>
+      <c r="B184" t="s">
+        <v>462</v>
+      </c>
+      <c r="C184" t="s">
+        <v>209</v>
+      </c>
+      <c r="D184" t="s">
+        <v>217</v>
+      </c>
+      <c r="E184" t="s">
+        <v>211</v>
+      </c>
+      <c r="F184" t="s">
+        <v>223</v>
+      </c>
+      <c r="G184" t="s">
+        <v>218</v>
+      </c>
+      <c r="H184" t="s">
+        <v>223</v>
+      </c>
+      <c r="I184" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9">
+      <c r="A185" t="s">
+        <v>463</v>
+      </c>
+      <c r="B185" t="s">
+        <v>464</v>
+      </c>
+      <c r="C185" t="s">
+        <v>209</v>
+      </c>
+      <c r="D185" t="s">
+        <v>217</v>
+      </c>
+      <c r="E185" t="s">
+        <v>211</v>
+      </c>
+      <c r="F185" t="s">
+        <v>223</v>
+      </c>
+      <c r="G185" t="s">
+        <v>218</v>
+      </c>
+      <c r="H185" t="s">
+        <v>223</v>
+      </c>
+      <c r="I185" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9">
+      <c r="A186" t="s">
+        <v>465</v>
+      </c>
+      <c r="B186" t="s">
+        <v>466</v>
+      </c>
+      <c r="C186" t="s">
+        <v>209</v>
+      </c>
+      <c r="D186" t="s">
+        <v>217</v>
+      </c>
+      <c r="E186" t="s">
+        <v>211</v>
+      </c>
+      <c r="F186" t="s">
+        <v>223</v>
+      </c>
+      <c r="G186" t="s">
+        <v>218</v>
+      </c>
+      <c r="H186" t="s">
+        <v>223</v>
+      </c>
+      <c r="I186" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9">
+      <c r="A187" t="s">
+        <v>467</v>
+      </c>
+      <c r="B187" t="s">
+        <v>468</v>
+      </c>
+      <c r="C187" t="s">
+        <v>209</v>
+      </c>
+      <c r="D187" t="s">
+        <v>217</v>
+      </c>
+      <c r="E187" t="s">
+        <v>211</v>
+      </c>
+      <c r="F187" t="s">
+        <v>223</v>
+      </c>
+      <c r="G187" t="s">
+        <v>218</v>
+      </c>
+      <c r="H187" t="s">
+        <v>223</v>
+      </c>
+      <c r="I187" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9">
+      <c r="A188" t="s">
+        <v>469</v>
+      </c>
+      <c r="B188" t="s">
+        <v>470</v>
+      </c>
+      <c r="C188" t="s">
+        <v>209</v>
+      </c>
+      <c r="D188" t="s">
+        <v>257</v>
+      </c>
+      <c r="E188" t="s">
+        <v>211</v>
+      </c>
+      <c r="F188" t="s">
+        <v>223</v>
+      </c>
+      <c r="G188" t="s">
+        <v>218</v>
+      </c>
+      <c r="H188" t="s">
+        <v>212</v>
+      </c>
+      <c r="I188" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9">
+      <c r="A189" t="s">
+        <v>471</v>
+      </c>
+      <c r="B189" t="s">
+        <v>472</v>
+      </c>
+      <c r="C189" t="s">
+        <v>265</v>
+      </c>
+      <c r="D189" t="s">
+        <v>217</v>
+      </c>
+      <c r="E189" t="s">
+        <v>211</v>
+      </c>
+      <c r="F189" t="s">
+        <v>212</v>
+      </c>
+      <c r="G189" t="s">
+        <v>218</v>
+      </c>
+      <c r="H189" t="s">
+        <v>223</v>
+      </c>
+      <c r="I189" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9">
+      <c r="A190" t="s">
+        <v>473</v>
+      </c>
+      <c r="B190" t="s">
+        <v>474</v>
+      </c>
+      <c r="C190" t="s">
+        <v>209</v>
+      </c>
+      <c r="D190" t="s">
+        <v>217</v>
+      </c>
+      <c r="E190" t="s">
+        <v>211</v>
+      </c>
+      <c r="F190" t="s">
+        <v>223</v>
+      </c>
+      <c r="G190" t="s">
+        <v>213</v>
+      </c>
+      <c r="H190" t="s">
+        <v>212</v>
+      </c>
+      <c r="I190" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9">
+      <c r="A191" t="s">
+        <v>475</v>
+      </c>
+      <c r="B191" t="s">
+        <v>476</v>
+      </c>
+      <c r="C191" t="s">
+        <v>209</v>
+      </c>
+      <c r="D191" t="s">
+        <v>217</v>
+      </c>
+      <c r="E191" t="s">
+        <v>211</v>
+      </c>
+      <c r="F191" t="s">
+        <v>223</v>
+      </c>
+      <c r="G191" t="s">
+        <v>218</v>
+      </c>
+      <c r="H191" t="s">
+        <v>212</v>
+      </c>
+      <c r="I191" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9">
+      <c r="A192" t="s">
+        <v>477</v>
+      </c>
+      <c r="B192" t="s">
+        <v>478</v>
+      </c>
+      <c r="C192" t="s">
+        <v>265</v>
+      </c>
+      <c r="D192" t="s">
+        <v>217</v>
+      </c>
+      <c r="E192" t="s">
+        <v>211</v>
+      </c>
+      <c r="F192" t="s">
+        <v>223</v>
+      </c>
+      <c r="G192" t="s">
+        <v>213</v>
+      </c>
+      <c r="H192" t="s">
+        <v>223</v>
+      </c>
+      <c r="I192" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9">
+      <c r="A193" t="s">
+        <v>479</v>
+      </c>
+      <c r="B193" t="s">
+        <v>480</v>
+      </c>
+      <c r="C193" t="s">
+        <v>209</v>
+      </c>
+      <c r="D193" t="s">
+        <v>217</v>
+      </c>
+      <c r="E193" t="s">
+        <v>211</v>
+      </c>
+      <c r="F193" t="s">
+        <v>212</v>
+      </c>
+      <c r="G193" t="s">
+        <v>218</v>
+      </c>
+      <c r="H193" t="s">
+        <v>212</v>
+      </c>
+      <c r="I193" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9">
+      <c r="A194" t="s">
+        <v>481</v>
+      </c>
+      <c r="B194" t="s">
+        <v>482</v>
+      </c>
+      <c r="C194" t="s">
+        <v>209</v>
+      </c>
+      <c r="D194" t="s">
+        <v>217</v>
+      </c>
+      <c r="E194" t="s">
+        <v>328</v>
+      </c>
+      <c r="F194" t="s">
+        <v>223</v>
+      </c>
+      <c r="G194" t="s">
+        <v>218</v>
+      </c>
+      <c r="H194" t="s">
+        <v>223</v>
+      </c>
+      <c r="I194" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9">
+      <c r="A195" t="s">
+        <v>483</v>
+      </c>
+      <c r="B195" t="s">
+        <v>484</v>
+      </c>
+      <c r="C195" t="s">
+        <v>265</v>
+      </c>
+      <c r="D195" t="s">
+        <v>217</v>
+      </c>
+      <c r="E195" t="s">
+        <v>211</v>
+      </c>
+      <c r="F195" t="s">
+        <v>223</v>
+      </c>
+      <c r="G195" t="s">
+        <v>218</v>
+      </c>
+      <c r="H195" t="s">
+        <v>223</v>
+      </c>
+      <c r="I195" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9">
+      <c r="A196" t="s">
+        <v>485</v>
+      </c>
+      <c r="B196" t="s">
+        <v>486</v>
+      </c>
+      <c r="C196" t="s">
+        <v>209</v>
+      </c>
+      <c r="D196" t="s">
+        <v>217</v>
+      </c>
+      <c r="E196" t="s">
+        <v>211</v>
+      </c>
+      <c r="F196" t="s">
+        <v>223</v>
+      </c>
+      <c r="G196" t="s">
+        <v>213</v>
+      </c>
+      <c r="H196" t="s">
+        <v>223</v>
+      </c>
+      <c r="I196" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9">
+      <c r="A197" t="s">
+        <v>487</v>
+      </c>
+      <c r="B197" t="s">
+        <v>488</v>
+      </c>
+      <c r="C197" t="s">
+        <v>209</v>
+      </c>
+      <c r="D197" t="s">
+        <v>217</v>
+      </c>
+      <c r="E197" t="s">
+        <v>211</v>
+      </c>
+      <c r="F197" t="s">
+        <v>212</v>
+      </c>
+      <c r="G197" t="s">
+        <v>218</v>
+      </c>
+      <c r="H197" t="s">
+        <v>223</v>
+      </c>
+      <c r="I197" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9">
+      <c r="A198" t="s">
+        <v>489</v>
+      </c>
+      <c r="B198" t="s">
+        <v>490</v>
+      </c>
+      <c r="C198" t="s">
+        <v>209</v>
+      </c>
+      <c r="D198" t="s">
+        <v>217</v>
+      </c>
+      <c r="E198" t="s">
+        <v>211</v>
+      </c>
+      <c r="F198" t="s">
+        <v>212</v>
+      </c>
+      <c r="G198" t="s">
+        <v>218</v>
+      </c>
+      <c r="H198" t="s">
+        <v>212</v>
+      </c>
+      <c r="I198" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9">
+      <c r="A199" t="s">
+        <v>491</v>
+      </c>
+      <c r="B199" t="s">
+        <v>492</v>
+      </c>
+      <c r="C199" t="s">
+        <v>209</v>
+      </c>
+      <c r="D199" t="s">
+        <v>217</v>
+      </c>
+      <c r="E199" t="s">
+        <v>211</v>
+      </c>
+      <c r="F199" t="s">
+        <v>212</v>
+      </c>
+      <c r="G199" t="s">
+        <v>218</v>
+      </c>
+      <c r="H199" t="s">
+        <v>223</v>
+      </c>
+      <c r="I199" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9">
+      <c r="A200" t="s">
+        <v>493</v>
+      </c>
+      <c r="B200" t="s">
+        <v>494</v>
+      </c>
+      <c r="C200" t="s">
+        <v>216</v>
+      </c>
+      <c r="D200" t="s">
+        <v>217</v>
+      </c>
+      <c r="E200" t="s">
+        <v>211</v>
+      </c>
+      <c r="F200" t="s">
+        <v>223</v>
+      </c>
+      <c r="G200" t="s">
+        <v>218</v>
+      </c>
+      <c r="H200" t="s">
+        <v>212</v>
+      </c>
+      <c r="I200" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9">
+      <c r="A201" t="s">
+        <v>495</v>
+      </c>
+      <c r="B201" t="s">
+        <v>496</v>
+      </c>
+      <c r="C201" t="s">
+        <v>209</v>
+      </c>
+      <c r="D201" t="s">
+        <v>217</v>
+      </c>
+      <c r="E201" t="s">
+        <v>211</v>
+      </c>
+      <c r="F201" t="s">
+        <v>212</v>
+      </c>
+      <c r="G201" t="s">
+        <v>218</v>
+      </c>
+      <c r="H201" t="s">
+        <v>223</v>
+      </c>
+      <c r="I201" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9">
+      <c r="A202" t="s">
+        <v>497</v>
+      </c>
+      <c r="B202" t="s">
+        <v>498</v>
+      </c>
+      <c r="C202" t="s">
+        <v>209</v>
+      </c>
+      <c r="D202" t="s">
+        <v>217</v>
+      </c>
+      <c r="E202" t="s">
+        <v>211</v>
+      </c>
+      <c r="F202" t="s">
+        <v>212</v>
+      </c>
+      <c r="G202" t="s">
+        <v>218</v>
+      </c>
+      <c r="H202" t="s">
+        <v>223</v>
+      </c>
+      <c r="I202" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9">
+      <c r="A203" t="s">
+        <v>499</v>
+      </c>
+      <c r="B203" t="s">
+        <v>500</v>
+      </c>
+      <c r="C203" t="s">
+        <v>209</v>
+      </c>
+      <c r="D203" t="s">
+        <v>217</v>
+      </c>
+      <c r="E203" t="s">
+        <v>211</v>
+      </c>
+      <c r="F203" t="s">
+        <v>223</v>
+      </c>
+      <c r="G203" t="s">
+        <v>213</v>
+      </c>
+      <c r="H203" t="s">
+        <v>223</v>
+      </c>
+      <c r="I203" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9">
+      <c r="A204" t="s">
+        <v>501</v>
+      </c>
+      <c r="B204" t="s">
+        <v>502</v>
+      </c>
+      <c r="C204" t="s">
+        <v>209</v>
+      </c>
+      <c r="D204" t="s">
+        <v>217</v>
+      </c>
+      <c r="E204" t="s">
+        <v>211</v>
+      </c>
+      <c r="F204" t="s">
+        <v>223</v>
+      </c>
+      <c r="G204" t="s">
+        <v>218</v>
+      </c>
+      <c r="H204" t="s">
+        <v>212</v>
+      </c>
+      <c r="I204" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9">
+      <c r="A205" t="s">
+        <v>503</v>
+      </c>
+      <c r="B205" t="s">
+        <v>504</v>
+      </c>
+      <c r="C205" t="s">
+        <v>209</v>
+      </c>
+      <c r="D205" t="s">
+        <v>217</v>
+      </c>
+      <c r="E205" t="s">
+        <v>211</v>
+      </c>
+      <c r="F205" t="s">
+        <v>223</v>
+      </c>
+      <c r="G205" t="s">
+        <v>218</v>
+      </c>
+      <c r="H205" t="s">
+        <v>212</v>
+      </c>
+      <c r="I205" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9">
+      <c r="A206" t="s">
+        <v>505</v>
+      </c>
+      <c r="B206" t="s">
+        <v>506</v>
+      </c>
+      <c r="C206" t="s">
+        <v>209</v>
+      </c>
+      <c r="D206" t="s">
+        <v>217</v>
+      </c>
+      <c r="E206" t="s">
+        <v>272</v>
+      </c>
+      <c r="F206" t="s">
+        <v>223</v>
+      </c>
+      <c r="G206" t="s">
+        <v>213</v>
+      </c>
+      <c r="H206" t="s">
+        <v>223</v>
+      </c>
+      <c r="I206" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9">
+      <c r="A207" t="s">
+        <v>507</v>
+      </c>
+      <c r="B207" t="s">
+        <v>508</v>
+      </c>
+      <c r="C207" t="s">
+        <v>209</v>
+      </c>
+      <c r="D207" t="s">
+        <v>210</v>
+      </c>
+      <c r="E207" t="s">
+        <v>211</v>
+      </c>
+      <c r="F207" t="s">
+        <v>212</v>
+      </c>
+      <c r="G207" t="s">
+        <v>213</v>
+      </c>
+      <c r="H207" t="s">
+        <v>223</v>
+      </c>
+      <c r="I207" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9">
+      <c r="A208" t="s">
+        <v>509</v>
+      </c>
+      <c r="B208" t="s">
+        <v>510</v>
+      </c>
+      <c r="C208" t="s">
+        <v>209</v>
+      </c>
+      <c r="D208" t="s">
+        <v>217</v>
+      </c>
+      <c r="E208" t="s">
+        <v>211</v>
+      </c>
+      <c r="F208" t="s">
+        <v>223</v>
+      </c>
+      <c r="G208" t="s">
+        <v>218</v>
+      </c>
+      <c r="H208" t="s">
+        <v>223</v>
+      </c>
+      <c r="I208" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9">
+      <c r="A209" t="s">
+        <v>511</v>
+      </c>
+      <c r="B209" t="s">
+        <v>512</v>
+      </c>
+      <c r="C209" t="s">
+        <v>265</v>
+      </c>
+      <c r="D209" t="s">
+        <v>217</v>
+      </c>
+      <c r="E209" t="s">
+        <v>272</v>
+      </c>
+      <c r="F209" t="s">
+        <v>223</v>
+      </c>
+      <c r="G209" t="s">
+        <v>218</v>
+      </c>
+      <c r="H209" t="s">
+        <v>223</v>
+      </c>
+      <c r="I209" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9">
+      <c r="A210" t="s">
+        <v>513</v>
+      </c>
+      <c r="B210" t="s">
+        <v>514</v>
+      </c>
+      <c r="C210" t="s">
+        <v>209</v>
+      </c>
+      <c r="D210" t="s">
+        <v>217</v>
+      </c>
+      <c r="E210" t="s">
+        <v>211</v>
+      </c>
+      <c r="F210" t="s">
+        <v>223</v>
+      </c>
+      <c r="G210" t="s">
+        <v>218</v>
+      </c>
+      <c r="H210" t="s">
+        <v>223</v>
+      </c>
+      <c r="I210" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9">
+      <c r="A211" t="s">
+        <v>515</v>
+      </c>
+      <c r="B211" t="s">
+        <v>516</v>
+      </c>
+      <c r="C211" t="s">
+        <v>209</v>
+      </c>
+      <c r="D211" t="s">
+        <v>217</v>
+      </c>
+      <c r="E211" t="s">
+        <v>272</v>
+      </c>
+      <c r="F211" t="s">
+        <v>212</v>
+      </c>
+      <c r="G211" t="s">
+        <v>213</v>
+      </c>
+      <c r="H211" t="s">
+        <v>223</v>
+      </c>
+      <c r="I211" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9">
+      <c r="A212" t="s">
+        <v>517</v>
+      </c>
+      <c r="B212" t="s">
+        <v>518</v>
+      </c>
+      <c r="C212" t="s">
+        <v>209</v>
+      </c>
+      <c r="D212" t="s">
+        <v>217</v>
+      </c>
+      <c r="E212" t="s">
+        <v>211</v>
+      </c>
+      <c r="F212" t="s">
+        <v>223</v>
+      </c>
+      <c r="G212" t="s">
+        <v>218</v>
+      </c>
+      <c r="H212" t="s">
+        <v>223</v>
+      </c>
+      <c r="I212" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9">
+      <c r="A213" t="s">
+        <v>519</v>
+      </c>
+      <c r="B213" t="s">
+        <v>520</v>
+      </c>
+      <c r="C213" t="s">
+        <v>209</v>
+      </c>
+      <c r="D213" t="s">
+        <v>217</v>
+      </c>
+      <c r="E213" t="s">
+        <v>211</v>
+      </c>
+      <c r="F213" t="s">
+        <v>223</v>
+      </c>
+      <c r="G213" t="s">
+        <v>213</v>
+      </c>
+      <c r="H213" t="s">
+        <v>223</v>
+      </c>
+      <c r="I213" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9">
+      <c r="A214" t="s">
+        <v>521</v>
+      </c>
+      <c r="B214" t="s">
+        <v>522</v>
+      </c>
+      <c r="C214" t="s">
+        <v>209</v>
+      </c>
+      <c r="D214" t="s">
+        <v>217</v>
+      </c>
+      <c r="E214" t="s">
+        <v>211</v>
+      </c>
+      <c r="F214" t="s">
+        <v>223</v>
+      </c>
+      <c r="G214" t="s">
+        <v>218</v>
+      </c>
+      <c r="H214" t="s">
+        <v>223</v>
+      </c>
+      <c r="I214" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9">
+      <c r="A215" t="s">
+        <v>523</v>
+      </c>
+      <c r="B215" t="s">
+        <v>524</v>
+      </c>
+      <c r="C215" t="s">
+        <v>209</v>
+      </c>
+      <c r="D215" t="s">
+        <v>217</v>
+      </c>
+      <c r="E215" t="s">
+        <v>211</v>
+      </c>
+      <c r="F215" t="s">
+        <v>212</v>
+      </c>
+      <c r="G215" t="s">
+        <v>213</v>
+      </c>
+      <c r="H215" t="s">
+        <v>223</v>
+      </c>
+      <c r="I215" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9">
+      <c r="A216" t="s">
+        <v>525</v>
+      </c>
+      <c r="B216" t="s">
+        <v>526</v>
+      </c>
+      <c r="C216" t="s">
+        <v>265</v>
+      </c>
+      <c r="D216" t="s">
+        <v>217</v>
+      </c>
+      <c r="E216" t="s">
+        <v>211</v>
+      </c>
+      <c r="F216" t="s">
+        <v>223</v>
+      </c>
+      <c r="G216" t="s">
+        <v>218</v>
+      </c>
+      <c r="H216" t="s">
+        <v>223</v>
+      </c>
+      <c r="I216" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9">
+      <c r="A217" t="s">
+        <v>527</v>
+      </c>
+      <c r="B217" t="s">
+        <v>528</v>
+      </c>
+      <c r="C217" t="s">
+        <v>209</v>
+      </c>
+      <c r="D217" t="s">
+        <v>257</v>
+      </c>
+      <c r="E217" t="s">
+        <v>211</v>
+      </c>
+      <c r="F217" t="s">
+        <v>223</v>
+      </c>
+      <c r="G217" t="s">
+        <v>213</v>
+      </c>
+      <c r="H217" t="s">
+        <v>223</v>
+      </c>
+      <c r="I217" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9">
+      <c r="A218" t="s">
+        <v>529</v>
+      </c>
+      <c r="B218" t="s">
+        <v>530</v>
+      </c>
+      <c r="C218" t="s">
+        <v>209</v>
+      </c>
+      <c r="D218" t="s">
+        <v>217</v>
+      </c>
+      <c r="E218" t="s">
+        <v>211</v>
+      </c>
+      <c r="F218" t="s">
+        <v>223</v>
+      </c>
+      <c r="G218" t="s">
+        <v>218</v>
+      </c>
+      <c r="H218" t="s">
+        <v>223</v>
+      </c>
+      <c r="I218" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9">
+      <c r="A219" t="s">
+        <v>531</v>
+      </c>
+      <c r="B219" t="s">
+        <v>532</v>
+      </c>
+      <c r="C219" t="s">
+        <v>265</v>
+      </c>
+      <c r="D219" t="s">
+        <v>217</v>
+      </c>
+      <c r="E219" t="s">
+        <v>211</v>
+      </c>
+      <c r="F219" t="s">
+        <v>212</v>
+      </c>
+      <c r="G219" t="s">
+        <v>213</v>
+      </c>
+      <c r="H219" t="s">
+        <v>223</v>
+      </c>
+      <c r="I219" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9">
+      <c r="A220" t="s">
+        <v>533</v>
+      </c>
+      <c r="B220" t="s">
+        <v>534</v>
+      </c>
+      <c r="C220" t="s">
+        <v>209</v>
+      </c>
+      <c r="D220" t="s">
+        <v>210</v>
+      </c>
+      <c r="E220" t="s">
+        <v>211</v>
+      </c>
+      <c r="F220" t="s">
+        <v>223</v>
+      </c>
+      <c r="G220" t="s">
+        <v>213</v>
+      </c>
+      <c r="H220" t="s">
+        <v>223</v>
+      </c>
+      <c r="I220" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>